<commit_message>
fix summary of capital gains
</commit_message>
<xml_diff>
--- a/example/report_2022_daily_rates.xlsx
+++ b/example/report_2022_daily_rates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="66">
   <si>
     <t>Symbol</t>
   </si>
@@ -45,7 +45,7 @@
     <t>Sell Price [EUR]</t>
   </si>
   <si>
-    <t>Total Gain [EUR]</t>
+    <t>Gain [EUR]</t>
   </si>
   <si>
     <t>NVDA</t>
@@ -57,9 +57,6 @@
     <t>GOOG</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>2019-02-28</t>
   </si>
   <si>
@@ -210,7 +207,7 @@
     <t>Zeile 20: In den Zeilen 18 und 19 enthaltene Gewinne aus Aktienveräußerungen i. S. d. § 20 Abs. 2 Satz 1 Nr 1 EStG</t>
   </si>
   <si>
-    <t>Zeile 23: In den Zeilen 18 und 19 enthaltene Verluste aus der Veräußerung aus der Veräuerung von Aktien i. S. d. § 20 Abs. 2 Satz 1 Nr. 1 EStG</t>
+    <t>Zeile 23: In den Zeilen 18 und 19 enthaltene Verluste aus der Veräuerung von Aktien i. S. d. § 20 Abs. 2 Satz 1 Nr. 1 EStG</t>
   </si>
   <si>
     <t>Zeile 41: Anrechenbare noch nicht angerechnete ausländische Steuern</t>
@@ -577,7 +574,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -620,16 +617,16 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2">
         <v>99.86</v>
@@ -649,16 +646,16 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3">
         <v>162.16</v>
@@ -678,16 +675,16 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4">
         <v>112.46</v>
@@ -707,16 +704,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5">
         <v>161.52</v>
@@ -736,16 +733,16 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6">
         <v>161.52</v>
@@ -765,16 +762,16 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7">
         <v>125.87</v>
@@ -794,16 +791,16 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G8">
         <v>125.87</v>
@@ -823,16 +820,16 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9">
         <v>91.54000000000001</v>
@@ -852,16 +849,16 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10">
         <v>91.54000000000001</v>
@@ -871,14 +868,6 @@
       </c>
       <c r="I10">
         <v>26.87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11">
-        <v>727.85</v>
       </c>
     </row>
   </sheetData>
@@ -888,7 +877,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -919,16 +908,16 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2">
         <v>0.9</v>
@@ -942,16 +931,16 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>85</v>
       </c>
       <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
         <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
       </c>
       <c r="E3">
         <v>0.96</v>
@@ -965,16 +954,16 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>3431.97</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4">
         <v>1.01</v>
@@ -988,16 +977,16 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>1825.99</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5">
         <v>1.01</v>
@@ -1011,16 +1000,16 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>3088.48</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6">
         <v>1.03</v>
@@ -1034,16 +1023,16 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7">
         <v>170</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7">
         <v>1.03</v>
@@ -1057,16 +1046,16 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8">
         <v>329.99</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8">
         <v>1.01</v>
@@ -1080,16 +1069,16 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>349.99</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9">
         <v>1.03</v>
@@ -1103,16 +1092,16 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>239.99</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10">
         <v>1.03</v>
@@ -1126,16 +1115,16 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>499.99</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11">
         <v>0.97</v>
@@ -1145,14 +1134,6 @@
       </c>
       <c r="G11">
         <v>-6.26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12">
-        <v>66.64</v>
       </c>
     </row>
   </sheetData>
@@ -1162,7 +1143,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1173,16 +1154,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1190,13 +1171,13 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2">
         <v>90.48</v>
@@ -1207,24 +1188,16 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3">
         <v>95.92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>186.4</v>
       </c>
     </row>
   </sheetData>
@@ -1234,7 +1207,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1245,30 +1218,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2">
         <v>0.03</v>
@@ -1276,16 +1249,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3">
         <v>0.01</v>
@@ -1293,16 +1266,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4">
         <v>0.02</v>
@@ -1310,16 +1283,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5">
         <v>15.45</v>
@@ -1327,16 +1300,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6">
         <v>0.01</v>
@@ -1344,16 +1317,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7">
         <v>0.01</v>
@@ -1361,16 +1334,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8">
         <v>0.01</v>
@@ -1378,16 +1351,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9">
         <v>0.01</v>
@@ -1395,27 +1368,19 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10">
         <v>14.35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11">
-        <v>29.9</v>
       </c>
     </row>
   </sheetData>
@@ -1425,7 +1390,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1436,16 +1401,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1453,13 +1418,13 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2">
         <v>13.57</v>
@@ -1470,24 +1435,16 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3">
         <v>14.39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>27.96</v>
       </c>
     </row>
   </sheetData>
@@ -1505,21 +1462,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2">
         <v>914.25</v>
@@ -1527,32 +1484,32 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3">
-        <v>727.85</v>
+        <v>974.86</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>247.01</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5">
         <v>27.96</v>
@@ -1560,10 +1517,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6">
         <v>29.9</v>
@@ -1571,10 +1528,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7">
         <v>66.64</v>

</xml_diff>

<commit_message>
Rename "wire_transfers" sheet to "currency conversion to EUR"
"Wire transfers" were a misnomer. It assumed that the currency
conversion happened on the very same day the wire transfer was initiated
(or finished) which was rarely the case.

Also, it carried a hidden notation that the user must have converted the
USD to EUR after a wire transfer which wasn't always the case.

Hence, the naming changed to be a lot more clear on the indended purpose
of the sheet.

Backwards compatibility was kept by still enabling reading from the old
sheet name with a warning message
</commit_message>
<xml_diff>
--- a/example/report_2022_daily_rates.xlsx
+++ b/example/report_2022_daily_rates.xlsx
@@ -168,7 +168,7 @@
     <t>Buying GOOG</t>
   </si>
   <si>
-    <t>Wire transfer</t>
+    <t>Currency conversion or wire transfer</t>
   </si>
   <si>
     <t>Selling APPL</t>
@@ -1058,7 +1058,7 @@
         <v>37</v>
       </c>
       <c r="B7">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -1073,7 +1073,7 @@
         <v>0.96</v>
       </c>
       <c r="G7">
-        <v>-11.67</v>
+        <v>-10.64</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1263,7 +1263,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -1629,7 +1629,7 @@
         <v>69</v>
       </c>
       <c r="C7">
-        <v>66.64</v>
+        <v>67.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add support for stock splits, use decimal.Decimal for better handling of floating point inputs
</commit_message>
<xml_diff>
--- a/example/report_2022_daily_rates.xlsx
+++ b/example/report_2022_daily_rates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="132">
   <si>
     <t>Symbol</t>
   </si>
@@ -57,18 +57,33 @@
     <t>GOOG</t>
   </si>
   <si>
+    <t>8.00</t>
+  </si>
+  <si>
+    <t>14.00</t>
+  </si>
+  <si>
+    <t>11.00</t>
+  </si>
+  <si>
+    <t>19.00</t>
+  </si>
+  <si>
+    <t>3.00</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>5.00</t>
+  </si>
+  <si>
     <t>2019-02-28</t>
   </si>
   <si>
     <t>2020-02-28</t>
   </si>
   <si>
-    <t>2021-09-21</t>
-  </si>
-  <si>
-    <t>2022-09-21</t>
-  </si>
-  <si>
     <t>2019-10-11</t>
   </si>
   <si>
@@ -93,16 +108,10 @@
     <t>2022-11-14</t>
   </si>
   <si>
-    <t>114.00 USD</t>
-  </si>
-  <si>
-    <t>178.00 USD</t>
-  </si>
-  <si>
-    <t>132.00 USD</t>
-  </si>
-  <si>
-    <t>160.00 USD</t>
+    <t>28.50 USD</t>
+  </si>
+  <si>
+    <t>44.50 USD</t>
   </si>
   <si>
     <t>139.00 USD</t>
@@ -132,9 +141,93 @@
     <t>100.00 USD</t>
   </si>
   <si>
+    <t>24.96</t>
+  </si>
+  <si>
+    <t>40.54</t>
+  </si>
+  <si>
+    <t>125.87</t>
+  </si>
+  <si>
+    <t>91.54</t>
+  </si>
+  <si>
+    <t>157.26</t>
+  </si>
+  <si>
+    <t>167.95</t>
+  </si>
+  <si>
+    <t>175.83</t>
+  </si>
+  <si>
+    <t>111.02</t>
+  </si>
+  <si>
+    <t>123.04</t>
+  </si>
+  <si>
+    <t>71.77</t>
+  </si>
+  <si>
+    <t>96.91</t>
+  </si>
+  <si>
+    <t>1058.34</t>
+  </si>
+  <si>
+    <t>1634.06</t>
+  </si>
+  <si>
+    <t>1401.50</t>
+  </si>
+  <si>
+    <t>2570.43</t>
+  </si>
+  <si>
+    <t>-44.55</t>
+  </si>
+  <si>
+    <t>-5.67</t>
+  </si>
+  <si>
+    <t>-98.81</t>
+  </si>
+  <si>
+    <t>26.87</t>
+  </si>
+  <si>
     <t>USD</t>
   </si>
   <si>
+    <t>85.00</t>
+  </si>
+  <si>
+    <t>3431.97</t>
+  </si>
+  <si>
+    <t>1825.99</t>
+  </si>
+  <si>
+    <t>3088.48</t>
+  </si>
+  <si>
+    <t>155.00</t>
+  </si>
+  <si>
+    <t>329.99</t>
+  </si>
+  <si>
+    <t>349.99</t>
+  </si>
+  <si>
+    <t>239.99</t>
+  </si>
+  <si>
+    <t>499.99</t>
+  </si>
+  <si>
     <t>2022-04-01</t>
   </si>
   <si>
@@ -147,6 +240,51 @@
     <t>2022-12-01</t>
   </si>
   <si>
+    <t>0.90</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>1.01</t>
+  </si>
+  <si>
+    <t>1.03</t>
+  </si>
+  <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>10.67</t>
+  </si>
+  <si>
+    <t>6.04</t>
+  </si>
+  <si>
+    <t>76.28</t>
+  </si>
+  <si>
+    <t>33.88</t>
+  </si>
+  <si>
+    <t>15.66</t>
+  </si>
+  <si>
+    <t>-10.64</t>
+  </si>
+  <si>
+    <t>-17.40</t>
+  </si>
+  <si>
+    <t>-24.06</t>
+  </si>
+  <si>
+    <t>-16.50</t>
+  </si>
+  <si>
+    <t>-6.26</t>
+  </si>
+  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -162,6 +300,12 @@
     <t>Dividend Payment</t>
   </si>
   <si>
+    <t>90.48</t>
+  </si>
+  <si>
+    <t>95.92</t>
+  </si>
+  <si>
     <t>Selling NVDA</t>
   </si>
   <si>
@@ -192,9 +336,33 @@
     <t>15.00 USD</t>
   </si>
   <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>5.14</t>
+  </si>
+  <si>
+    <t>15.45</t>
+  </si>
+  <si>
+    <t>14.35</t>
+  </si>
+  <si>
     <t>Withheld Tax on Dividends</t>
   </si>
   <si>
+    <t>13.57</t>
+  </si>
+  <si>
+    <t>14.39</t>
+  </si>
+  <si>
     <t>ELSTER - Anlage</t>
   </si>
   <si>
@@ -229,6 +397,24 @@
   </si>
   <si>
     <t>Zeilen 42 - 48: Gewinn / Verlust aus Verkauf von Fremdwährungen</t>
+  </si>
+  <si>
+    <t>6728.57</t>
+  </si>
+  <si>
+    <t>6691.20</t>
+  </si>
+  <si>
+    <t>149.03</t>
+  </si>
+  <si>
+    <t>27.96</t>
+  </si>
+  <si>
+    <t>35.04</t>
+  </si>
+  <si>
+    <t>67.67</t>
   </si>
 </sst>
 </file>
@@ -586,7 +772,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -633,261 +819,232 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
-        <v>2</v>
+      <c r="B2" t="s">
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2">
-        <v>99.86</v>
-      </c>
-      <c r="H2">
-        <v>157.26</v>
-      </c>
-      <c r="I2">
-        <v>114.8</v>
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3">
-        <v>162.16</v>
-      </c>
-      <c r="H3">
-        <v>157.26</v>
-      </c>
-      <c r="I3">
-        <v>-97.98</v>
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>10</v>
+      <c r="B4" t="s">
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4">
-        <v>112.46</v>
-      </c>
-      <c r="H4">
-        <v>167.95</v>
-      </c>
-      <c r="I4">
-        <v>554.9299999999999</v>
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
-        <v>1</v>
+      <c r="B5" t="s">
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5">
-        <v>161.52</v>
-      </c>
-      <c r="H5">
-        <v>167.95</v>
-      </c>
-      <c r="I5">
-        <v>6.43</v>
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6">
-        <v>161.52</v>
-      </c>
-      <c r="H6">
-        <v>175.83</v>
-      </c>
-      <c r="I6">
-        <v>271.83</v>
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>3</v>
+      <c r="B7" t="s">
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7">
-        <v>125.87</v>
-      </c>
-      <c r="H7">
-        <v>111.02</v>
-      </c>
-      <c r="I7">
-        <v>-44.55</v>
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8">
-        <v>125.87</v>
-      </c>
-      <c r="H8">
-        <v>123.04</v>
-      </c>
-      <c r="I8">
-        <v>-5.67</v>
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
-        <v>5</v>
+      <c r="B9" t="s">
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9">
-        <v>91.54000000000001</v>
-      </c>
-      <c r="H9">
-        <v>71.77</v>
-      </c>
-      <c r="I9">
-        <v>-98.81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10">
-        <v>91.54000000000001</v>
-      </c>
-      <c r="H10">
-        <v>96.91</v>
-      </c>
-      <c r="I10">
-        <v>26.87</v>
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -940,232 +1097,232 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2">
-        <v>85</v>
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2">
-        <v>0.9</v>
-      </c>
-      <c r="F2">
-        <v>1.03</v>
-      </c>
-      <c r="G2">
-        <v>10.67</v>
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3">
-        <v>85</v>
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3">
-        <v>0.96</v>
-      </c>
-      <c r="F3">
-        <v>1.03</v>
-      </c>
-      <c r="G3">
-        <v>6.04</v>
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4">
-        <v>3431.97</v>
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4">
-        <v>1.01</v>
-      </c>
-      <c r="F4">
-        <v>1.03</v>
-      </c>
-      <c r="G4">
-        <v>76.28</v>
+        <v>71</v>
+      </c>
+      <c r="E4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5">
-        <v>1825.99</v>
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5">
-        <v>1.01</v>
-      </c>
-      <c r="F5">
-        <v>1.03</v>
-      </c>
-      <c r="G5">
-        <v>33.88</v>
+        <v>71</v>
+      </c>
+      <c r="E5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6">
-        <v>3088.48</v>
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6">
-        <v>1.03</v>
-      </c>
-      <c r="F6">
-        <v>1.03</v>
-      </c>
-      <c r="G6">
-        <v>15.66</v>
+        <v>71</v>
+      </c>
+      <c r="E6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7">
-        <v>155</v>
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7">
-        <v>1.03</v>
-      </c>
-      <c r="F7">
-        <v>0.96</v>
-      </c>
-      <c r="G7">
-        <v>-10.64</v>
+        <v>72</v>
+      </c>
+      <c r="E7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8">
-        <v>329.99</v>
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8">
-        <v>1.01</v>
-      </c>
-      <c r="F8">
-        <v>0.96</v>
-      </c>
-      <c r="G8">
-        <v>-17.4</v>
+        <v>72</v>
+      </c>
+      <c r="E8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9">
-        <v>349.99</v>
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9">
-        <v>1.03</v>
-      </c>
-      <c r="F9">
-        <v>0.96</v>
-      </c>
-      <c r="G9">
-        <v>-24.06</v>
+        <v>72</v>
+      </c>
+      <c r="E9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10">
-        <v>239.99</v>
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10">
-        <v>1.03</v>
-      </c>
-      <c r="F10">
-        <v>0.96</v>
-      </c>
-      <c r="G10">
-        <v>-16.5</v>
+        <v>72</v>
+      </c>
+      <c r="E10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11">
-        <v>499.99</v>
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11">
-        <v>0.97</v>
-      </c>
-      <c r="F11">
-        <v>0.96</v>
-      </c>
-      <c r="G11">
-        <v>-6.26</v>
+        <v>72</v>
+      </c>
+      <c r="E11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1198,16 +1355,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1215,16 +1372,16 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2">
-        <v>90.48</v>
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1232,16 +1389,16 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3">
-        <v>95.92</v>
+      <c r="E3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1274,186 +1431,186 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2">
-        <v>0.03</v>
+        <v>100</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3">
-        <v>0.01</v>
+        <v>101</v>
+      </c>
+      <c r="E3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4">
-        <v>0.02</v>
+        <v>102</v>
+      </c>
+      <c r="E4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5">
-        <v>5.14</v>
+        <v>103</v>
+      </c>
+      <c r="E5" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6">
-        <v>15.45</v>
+        <v>104</v>
+      </c>
+      <c r="E6" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7">
-        <v>0.01</v>
+        <v>101</v>
+      </c>
+      <c r="E7" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8">
-        <v>0.01</v>
+        <v>101</v>
+      </c>
+      <c r="E8" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9">
-        <v>0.01</v>
+        <v>101</v>
+      </c>
+      <c r="E9" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10">
-        <v>0.01</v>
+        <v>101</v>
+      </c>
+      <c r="E10" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11">
-        <v>14.35</v>
+        <v>104</v>
+      </c>
+      <c r="E11" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1486,16 +1643,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1503,16 +1660,16 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2">
-        <v>13.57</v>
+        <v>104</v>
+      </c>
+      <c r="E2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1520,16 +1677,16 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3">
-        <v>14.39</v>
+        <v>104</v>
+      </c>
+      <c r="E3" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1552,84 +1709,84 @@
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="105.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2">
-        <v>914.25</v>
+        <v>120</v>
+      </c>
+      <c r="C2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3">
-        <v>974.86</v>
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4">
-        <v>247.01</v>
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5">
-        <v>27.96</v>
+        <v>123</v>
+      </c>
+      <c r="C5" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6">
-        <v>35.04</v>
+        <v>124</v>
+      </c>
+      <c r="C6" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7">
-        <v>67.67</v>
+        <v>125</v>
+      </c>
+      <c r="C7" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add explicit tab for currency movements, fix typing hints and other minor issues
</commit_message>
<xml_diff>
--- a/example/report_2022_daily_rates.xlsx
+++ b/example/report_2022_daily_rates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="141">
   <si>
     <t>Symbol</t>
   </si>
@@ -48,6 +48,18 @@
     <t>Gain [EUR]</t>
   </si>
   <si>
+    <t>---------------------</t>
+  </si>
+  <si>
+    <t>Gains (incl. losses)</t>
+  </si>
+  <si>
+    <t>Gains (excl. losses)</t>
+  </si>
+  <si>
+    <t>Losses</t>
+  </si>
+  <si>
     <t>NVDA</t>
   </si>
   <si>
@@ -57,16 +69,25 @@
     <t>GOOG</t>
   </si>
   <si>
-    <t>---------------------</t>
-  </si>
-  <si>
-    <t>Gains (incl. losses)</t>
-  </si>
-  <si>
-    <t>Gains (excl. losses)</t>
-  </si>
-  <si>
-    <t>Losses</t>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>20.00</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>19.00</t>
+  </si>
+  <si>
+    <t>3.00</t>
+  </si>
+  <si>
+    <t>5.00</t>
   </si>
   <si>
     <t>2019-02-28</t>
@@ -144,9 +165,111 @@
     <t>100.00 USD</t>
   </si>
   <si>
+    <t>99.86</t>
+  </si>
+  <si>
+    <t>162.16</t>
+  </si>
+  <si>
+    <t>112.46</t>
+  </si>
+  <si>
+    <t>161.52</t>
+  </si>
+  <si>
+    <t>125.87</t>
+  </si>
+  <si>
+    <t>91.54</t>
+  </si>
+  <si>
+    <t>157.26</t>
+  </si>
+  <si>
+    <t>167.95</t>
+  </si>
+  <si>
+    <t>175.83</t>
+  </si>
+  <si>
+    <t>111.02</t>
+  </si>
+  <si>
+    <t>123.04</t>
+  </si>
+  <si>
+    <t>71.77</t>
+  </si>
+  <si>
+    <t>96.91</t>
+  </si>
+  <si>
+    <t>727.85</t>
+  </si>
+  <si>
+    <t>974.86</t>
+  </si>
+  <si>
+    <t>-247.01</t>
+  </si>
+  <si>
+    <t>114.80</t>
+  </si>
+  <si>
+    <t>-97.98</t>
+  </si>
+  <si>
+    <t>554.93</t>
+  </si>
+  <si>
+    <t>6.43</t>
+  </si>
+  <si>
+    <t>271.83</t>
+  </si>
+  <si>
+    <t>-44.55</t>
+  </si>
+  <si>
+    <t>-5.67</t>
+  </si>
+  <si>
+    <t>-98.81</t>
+  </si>
+  <si>
+    <t>26.87</t>
+  </si>
+  <si>
     <t>USD</t>
   </si>
   <si>
+    <t>85.00</t>
+  </si>
+  <si>
+    <t>3431.97</t>
+  </si>
+  <si>
+    <t>1825.99</t>
+  </si>
+  <si>
+    <t>3088.48</t>
+  </si>
+  <si>
+    <t>170.00</t>
+  </si>
+  <si>
+    <t>329.99</t>
+  </si>
+  <si>
+    <t>349.99</t>
+  </si>
+  <si>
+    <t>239.99</t>
+  </si>
+  <si>
+    <t>499.99</t>
+  </si>
+  <si>
     <t>2022-04-01</t>
   </si>
   <si>
@@ -157,6 +280,60 @@
   </si>
   <si>
     <t>2022-12-01</t>
+  </si>
+  <si>
+    <t>0.90</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>1.01</t>
+  </si>
+  <si>
+    <t>1.03</t>
+  </si>
+  <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>66.64</t>
+  </si>
+  <si>
+    <t>142.53</t>
+  </si>
+  <si>
+    <t>-75.89</t>
+  </si>
+  <si>
+    <t>10.67</t>
+  </si>
+  <si>
+    <t>6.04</t>
+  </si>
+  <si>
+    <t>76.28</t>
+  </si>
+  <si>
+    <t>33.88</t>
+  </si>
+  <si>
+    <t>15.66</t>
+  </si>
+  <si>
+    <t>-11.67</t>
+  </si>
+  <si>
+    <t>-17.40</t>
+  </si>
+  <si>
+    <t>-24.06</t>
+  </si>
+  <si>
+    <t>-16.50</t>
+  </si>
+  <si>
+    <t>-6.26</t>
   </si>
   <si>
     <t>Comment</t>
@@ -669,290 +846,290 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2">
-        <v>99.86</v>
-      </c>
-      <c r="H2">
-        <v>157.26</v>
-      </c>
-      <c r="I2">
-        <v>114.8</v>
-      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3">
-        <v>162.16</v>
-      </c>
-      <c r="H3">
-        <v>157.26</v>
-      </c>
-      <c r="I3">
-        <v>-97.98</v>
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4">
-        <v>112.46</v>
-      </c>
-      <c r="H4">
-        <v>167.95</v>
-      </c>
-      <c r="I4">
-        <v>554.9299999999999</v>
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5">
-        <v>161.52</v>
-      </c>
-      <c r="H5">
-        <v>167.95</v>
-      </c>
-      <c r="I5">
-        <v>6.43</v>
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6">
-        <v>161.52</v>
-      </c>
-      <c r="H6">
-        <v>175.83</v>
-      </c>
-      <c r="I6">
-        <v>271.83</v>
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7">
-        <v>125.87</v>
-      </c>
-      <c r="H7">
-        <v>111.02</v>
-      </c>
-      <c r="I7">
-        <v>-44.55</v>
+        <v>41</v>
+      </c>
+      <c r="G7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8">
-        <v>125.87</v>
-      </c>
-      <c r="H8">
-        <v>123.04</v>
-      </c>
-      <c r="I8">
-        <v>-5.67</v>
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9">
-        <v>91.54000000000001</v>
-      </c>
-      <c r="H9">
-        <v>71.77</v>
-      </c>
-      <c r="I9">
-        <v>-98.81</v>
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10">
-        <v>91.54000000000001</v>
-      </c>
-      <c r="H10">
-        <v>96.91</v>
-      </c>
-      <c r="I10">
-        <v>26.87</v>
+        <v>43</v>
+      </c>
+      <c r="G10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12">
-        <v>727.85</v>
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13">
-        <v>974.86</v>
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="I14">
-        <v>-247.01</v>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1005,261 +1182,261 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2">
-        <v>85</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2">
-        <v>0.9</v>
-      </c>
-      <c r="F2">
-        <v>1.03</v>
-      </c>
-      <c r="G2">
-        <v>10.67</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3">
-        <v>85</v>
-      </c>
-      <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3">
-        <v>0.96</v>
-      </c>
-      <c r="F3">
-        <v>1.03</v>
-      </c>
-      <c r="G3">
-        <v>6.04</v>
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4">
-        <v>3431.97</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4">
-        <v>1.01</v>
-      </c>
-      <c r="F4">
-        <v>1.03</v>
-      </c>
-      <c r="G4">
-        <v>76.28</v>
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5">
-        <v>1825.99</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5">
-        <v>1.01</v>
-      </c>
-      <c r="F5">
-        <v>1.03</v>
-      </c>
-      <c r="G5">
-        <v>33.88</v>
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6">
-        <v>3088.48</v>
+        <v>73</v>
+      </c>
+      <c r="B6" t="s">
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6">
-        <v>1.03</v>
-      </c>
-      <c r="F6">
-        <v>1.03</v>
-      </c>
-      <c r="G6">
-        <v>15.66</v>
+        <v>85</v>
+      </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7">
-        <v>170</v>
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7">
-        <v>1.03</v>
-      </c>
-      <c r="F7">
-        <v>0.96</v>
-      </c>
-      <c r="G7">
-        <v>-11.67</v>
+        <v>85</v>
+      </c>
+      <c r="E7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8">
-        <v>329.99</v>
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8">
-        <v>1.01</v>
-      </c>
-      <c r="F8">
-        <v>0.96</v>
-      </c>
-      <c r="G8">
-        <v>-17.4</v>
+        <v>85</v>
+      </c>
+      <c r="E8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9">
-        <v>349.99</v>
+        <v>73</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9">
-        <v>1.03</v>
-      </c>
-      <c r="F9">
-        <v>0.96</v>
-      </c>
-      <c r="G9">
-        <v>-24.06</v>
+        <v>85</v>
+      </c>
+      <c r="E9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10">
-        <v>239.99</v>
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10">
-        <v>1.03</v>
-      </c>
-      <c r="F10">
-        <v>0.96</v>
-      </c>
-      <c r="G10">
-        <v>-16.5</v>
+        <v>85</v>
+      </c>
+      <c r="E10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11">
-        <v>499.99</v>
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11">
-        <v>0.97</v>
-      </c>
-      <c r="F11">
-        <v>0.96</v>
-      </c>
-      <c r="G11">
-        <v>-6.26</v>
+        <v>86</v>
+      </c>
+      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13">
-        <v>66.64</v>
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14">
-        <v>142.53</v>
+        <v>73</v>
+      </c>
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15">
-        <v>-75.89</v>
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1292,30 +1469,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E2">
         <v>90.48</v>
@@ -1323,16 +1500,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E3">
         <v>95.92</v>
@@ -1340,12 +1517,12 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
       <c r="E5">
         <v>186.4</v>
@@ -1381,30 +1558,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="E2">
         <v>0.03</v>
@@ -1412,16 +1589,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="E3">
         <v>0.01</v>
@@ -1429,16 +1606,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="E4">
         <v>0.02</v>
@@ -1446,16 +1623,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="E5">
         <v>15.45</v>
@@ -1463,16 +1640,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="E6">
         <v>0.01</v>
@@ -1480,16 +1657,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="E7">
         <v>0.01</v>
@@ -1497,16 +1674,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="E8">
         <v>0.01</v>
@@ -1514,16 +1691,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="E9">
         <v>0.01</v>
@@ -1531,16 +1708,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="E10">
         <v>14.35</v>
@@ -1548,12 +1725,12 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
       <c r="E12">
         <v>29.9</v>
@@ -1589,30 +1766,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="E2">
         <v>13.57</v>
@@ -1620,16 +1797,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="E3">
         <v>14.39</v>
@@ -1637,12 +1814,12 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
       <c r="E5">
         <v>27.96</v>
@@ -1673,21 +1850,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>135</v>
       </c>
       <c r="C2">
         <v>914.25</v>
@@ -1695,10 +1872,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="C3">
         <v>974.86</v>
@@ -1706,10 +1883,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>137</v>
       </c>
       <c r="C4">
         <v>247.01</v>
@@ -1717,10 +1894,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>138</v>
       </c>
       <c r="C5">
         <v>27.96</v>
@@ -1728,10 +1905,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="C6">
         <v>29.9</v>
@@ -1739,10 +1916,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>140</v>
       </c>
       <c r="C7">
         <v>66.64</v>

</xml_diff>